<commit_message>
Component 2d Plan - 02
I update New table
</commit_message>
<xml_diff>
--- a/Dataset/3D plans/images.xlsx
+++ b/Dataset/3D plans/images.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LENOVO\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Samith\Documents\GitHub\House-Plan-Master\Dataset\3D plans\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="36">
   <si>
     <t>Bed rooms</t>
   </si>
@@ -41,28 +41,103 @@
     <t>Images</t>
   </si>
   <si>
-    <t>P12,P13</t>
-  </si>
-  <si>
-    <t>B2,B3,B6,B7,B7</t>
-  </si>
-  <si>
-    <t>B1,B4,B5,B9</t>
-  </si>
-  <si>
-    <t>P1,P2,P3,P4,P5,P6,P7,P8,P9,P10,P11</t>
-  </si>
-  <si>
-    <t>R1,R2,R4,R5,R7,R8,R9</t>
-  </si>
-  <si>
-    <t>R3,R6,R10</t>
+    <t>P2</t>
+  </si>
+  <si>
+    <t>P3</t>
+  </si>
+  <si>
+    <t>P4</t>
+  </si>
+  <si>
+    <t>P5</t>
+  </si>
+  <si>
+    <t>P6</t>
+  </si>
+  <si>
+    <t>P7</t>
+  </si>
+  <si>
+    <t>P8</t>
+  </si>
+  <si>
+    <t>P9</t>
+  </si>
+  <si>
+    <t>P10</t>
+  </si>
+  <si>
+    <t>P11</t>
+  </si>
+  <si>
+    <t>P13</t>
+  </si>
+  <si>
+    <t>P12</t>
+  </si>
+  <si>
+    <t>P1</t>
+  </si>
+  <si>
+    <t>B4</t>
+  </si>
+  <si>
+    <t>B5</t>
+  </si>
+  <si>
+    <t>B9</t>
+  </si>
+  <si>
+    <t>B1</t>
+  </si>
+  <si>
+    <t>B3</t>
+  </si>
+  <si>
+    <t>B6</t>
+  </si>
+  <si>
+    <t>B7</t>
+  </si>
+  <si>
+    <t>B2</t>
+  </si>
+  <si>
+    <t>R6</t>
+  </si>
+  <si>
+    <t>R10</t>
+  </si>
+  <si>
+    <t>R2</t>
+  </si>
+  <si>
+    <t>R4</t>
+  </si>
+  <si>
+    <t>R5</t>
+  </si>
+  <si>
+    <t>R7</t>
+  </si>
+  <si>
+    <t>R8</t>
+  </si>
+  <si>
+    <t>R9</t>
+  </si>
+  <si>
+    <t>R1</t>
+  </si>
+  <si>
+    <t>R3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -374,10 +449,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:F7"/>
+  <dimension ref="B1:F33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="F39" sqref="F39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -386,7 +461,7 @@
     <col min="3" max="3" width="13.42578125" customWidth="1"/>
     <col min="4" max="4" width="12" customWidth="1"/>
     <col min="5" max="5" width="11.28515625" customWidth="1"/>
-    <col min="6" max="6" width="70.140625" customWidth="1"/>
+    <col min="6" max="6" width="16.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:6" x14ac:dyDescent="0.25">
@@ -420,7 +495,7 @@
         <v>1</v>
       </c>
       <c r="F2" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.25">
@@ -428,7 +503,7 @@
         <v>1</v>
       </c>
       <c r="C3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -442,7 +517,7 @@
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -454,15 +529,15 @@
         <v>1</v>
       </c>
       <c r="F4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -471,12 +546,12 @@
         <v>1</v>
       </c>
       <c r="F5" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B6">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -488,15 +563,15 @@
         <v>1</v>
       </c>
       <c r="F6" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B7">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D7">
         <v>1</v>
@@ -506,6 +581,448 @@
       </c>
       <c r="F7" t="s">
         <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="F12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13">
+        <v>2</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+      <c r="F13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14">
+        <v>2</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+      <c r="F14" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B15">
+        <v>2</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15">
+        <v>1</v>
+      </c>
+      <c r="F15" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B16">
+        <v>2</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
+      <c r="F16" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B17">
+        <v>2</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="E17">
+        <v>1</v>
+      </c>
+      <c r="F17" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B18">
+        <v>2</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
+      <c r="E18">
+        <v>1</v>
+      </c>
+      <c r="F18" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B19">
+        <v>2</v>
+      </c>
+      <c r="C19">
+        <v>2</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+      <c r="E19">
+        <v>1</v>
+      </c>
+      <c r="F19" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B20">
+        <v>2</v>
+      </c>
+      <c r="C20">
+        <v>2</v>
+      </c>
+      <c r="D20">
+        <v>1</v>
+      </c>
+      <c r="E20">
+        <v>1</v>
+      </c>
+      <c r="F20" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B21">
+        <v>2</v>
+      </c>
+      <c r="C21">
+        <v>2</v>
+      </c>
+      <c r="D21">
+        <v>1</v>
+      </c>
+      <c r="E21">
+        <v>1</v>
+      </c>
+      <c r="F21" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B22">
+        <v>2</v>
+      </c>
+      <c r="C22">
+        <v>2</v>
+      </c>
+      <c r="D22">
+        <v>1</v>
+      </c>
+      <c r="E22">
+        <v>1</v>
+      </c>
+      <c r="F22" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B23">
+        <v>2</v>
+      </c>
+      <c r="C23">
+        <v>2</v>
+      </c>
+      <c r="D23">
+        <v>1</v>
+      </c>
+      <c r="E23">
+        <v>1</v>
+      </c>
+      <c r="F23" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B24">
+        <v>3</v>
+      </c>
+      <c r="C24">
+        <v>1</v>
+      </c>
+      <c r="D24">
+        <v>1</v>
+      </c>
+      <c r="E24">
+        <v>1</v>
+      </c>
+      <c r="F24" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B25">
+        <v>3</v>
+      </c>
+      <c r="C25">
+        <v>1</v>
+      </c>
+      <c r="D25">
+        <v>1</v>
+      </c>
+      <c r="E25">
+        <v>1</v>
+      </c>
+      <c r="F25" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B26">
+        <v>3</v>
+      </c>
+      <c r="C26">
+        <v>1</v>
+      </c>
+      <c r="D26">
+        <v>1</v>
+      </c>
+      <c r="E26">
+        <v>1</v>
+      </c>
+      <c r="F26" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B27">
+        <v>3</v>
+      </c>
+      <c r="C27">
+        <v>2</v>
+      </c>
+      <c r="D27">
+        <v>1</v>
+      </c>
+      <c r="E27">
+        <v>1</v>
+      </c>
+      <c r="F27" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B28">
+        <v>3</v>
+      </c>
+      <c r="C28">
+        <v>2</v>
+      </c>
+      <c r="D28">
+        <v>1</v>
+      </c>
+      <c r="E28">
+        <v>1</v>
+      </c>
+      <c r="F28" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B29">
+        <v>3</v>
+      </c>
+      <c r="C29">
+        <v>2</v>
+      </c>
+      <c r="D29">
+        <v>1</v>
+      </c>
+      <c r="E29">
+        <v>1</v>
+      </c>
+      <c r="F29" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B30">
+        <v>3</v>
+      </c>
+      <c r="C30">
+        <v>2</v>
+      </c>
+      <c r="D30">
+        <v>1</v>
+      </c>
+      <c r="E30">
+        <v>1</v>
+      </c>
+      <c r="F30" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B31">
+        <v>3</v>
+      </c>
+      <c r="C31">
+        <v>2</v>
+      </c>
+      <c r="D31">
+        <v>1</v>
+      </c>
+      <c r="E31">
+        <v>1</v>
+      </c>
+      <c r="F31" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B32">
+        <v>3</v>
+      </c>
+      <c r="C32">
+        <v>2</v>
+      </c>
+      <c r="D32">
+        <v>1</v>
+      </c>
+      <c r="E32">
+        <v>1</v>
+      </c>
+      <c r="F32" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B33">
+        <v>3</v>
+      </c>
+      <c r="C33">
+        <v>2</v>
+      </c>
+      <c r="D33">
+        <v>1</v>
+      </c>
+      <c r="E33">
+        <v>1</v>
+      </c>
+      <c r="F33" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>